<commit_message>
Add TrakTVLogin to Config
</commit_message>
<xml_diff>
--- a/Dispatcher/Data/Config.xlsx
+++ b/Dispatcher/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve">Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraktTVLogin</t>
   </si>
   <si>
     <t xml:space="preserve">MaxRetryNumber</t>
@@ -175,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -212,12 +215,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -283,7 +280,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -307,10 +304,10 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43"/>
@@ -386,7 +383,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1401,7 +1405,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51"/>
@@ -1445,136 +1449,136 @@
     </row>
     <row r="2" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2570,12 +2574,12 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="65.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="65.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2583,13 +2587,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2616,10 +2620,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Rename TraktTV Login Workflow, Add Browser Activities to it, Create SignOutofTraktTV Workflow
</commit_message>
<xml_diff>
--- a/Dispatcher/Data/Config.xlsx
+++ b/Dispatcher/Data/Config.xlsx
@@ -307,7 +307,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43"/>
@@ -1405,7 +1405,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51"/>
@@ -2574,7 +2574,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.1"/>

</xml_diff>